<commit_message>
Made second changes to the file
</commit_message>
<xml_diff>
--- a/PythonFunctions.xlsx
+++ b/PythonFunctions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Language Fundas" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="833">
   <si>
     <t>Function</t>
   </si>
@@ -2806,6 +2806,15 @@
   </si>
   <si>
     <t>'afkpu'</t>
+  </si>
+  <si>
+    <t>var[::-1]</t>
+  </si>
+  <si>
+    <t>[0:25:-1]</t>
+  </si>
+  <si>
+    <t>zyxwvutsrqponmlkjihgfedcba'</t>
   </si>
 </sst>
 </file>
@@ -2900,7 +2909,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2954,6 +2963,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3260,7 +3270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A39" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4505,10 +4515,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4774,6 +4784,17 @@
       </c>
       <c r="C25" t="s">
         <v>829</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>830</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>831</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>